<commit_message>
Funciona el login usando foreach
</commit_message>
<xml_diff>
--- a/excel/baseDatosExcel.xlsx
+++ b/excel/baseDatosExcel.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
-    <t>CÓDIGO</t>
+    <t>COD</t>
   </si>
   <si>
     <t>NOMBRES</t>
@@ -77,12 +77,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* \-??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -91,6 +91,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -99,10 +122,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -115,74 +138,67 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -196,49 +212,41 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -257,181 +265,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -445,17 +453,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -477,9 +479,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -517,19 +521,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -537,161 +530,179 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1078,7 +1089,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="3"/>
@@ -1087,20 +1098,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>101</v>
       </c>
@@ -1110,8 +1121,11 @@
       <c r="C2">
         <v>1</v>
       </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>102</v>
       </c>
@@ -1121,8 +1135,11 @@
       <c r="C3">
         <v>10</v>
       </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>103</v>
       </c>
@@ -1132,8 +1149,11 @@
       <c r="C4">
         <v>7</v>
       </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>104</v>
       </c>
@@ -1143,8 +1163,11 @@
       <c r="C5">
         <v>8</v>
       </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>105</v>
       </c>
@@ -1153,13 +1176,16 @@
       </c>
       <c r="C6">
         <v>9</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="A1:D1;A2:C2;A3:D3;A4;D4;A5;D5;A6;D6;B7:D21" numberStoredAsText="1"/>
+    <ignoredError sqref="B2;B3;C7:D21;C1:D1;C3;C2;B1;A2;A4;A5;A6;B7:B21;A3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>